<commit_message>
/resource/registrants/Freezed The 3rd K-PAI Seminar Application (Responses) - Form Responses 1.tsv/ update /resource/registrants/registrants.xlsx/ updated
</commit_message>
<xml_diff>
--- a/resource/registrants/registrants.xlsx
+++ b/resource/registrants/registrants.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5693,7 +5693,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>정재헌</t>
+          <t>정태희</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -5704,39 +5704,39 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>o</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>YC America</t>
+          <t>Waymo</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>President</t>
+          <t>Software Engineer</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>jae.jeong@yccorp.com</t>
+          <t>wwee3631@gmail.com</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>+1 408-209-0602</t>
+          <t>+1 669-977-9158</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>https:///linkedin.com/in/jae-jaeheon-jeong-39b99434</t>
+          <t>https://www.linkedin.com/in/taeheejeong/</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>정태희</t>
+          <t>정한솔</t>
         </is>
       </c>
       <c r="B137" t="inlineStr"/>
@@ -5752,34 +5752,34 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Waymo</t>
+          <t>Stanford University</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>wwee3631@gmail.com</t>
+          <t>hansol2@stanford.edu</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>+1 669-977-9158</t>
+          <t>+1 630-698-4717</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/taeheejeong/</t>
+          <t>https:///linkedin.com/in/esther-hansol-chung-071b9b19b</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>정한솔</t>
+          <t>정혜령</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
@@ -5790,39 +5790,39 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Stanford University</t>
+          <t>Samsung Electronics</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Sr. Marketing Communications Specialist</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>hansol2@stanford.edu</t>
+          <t>lydia.chung1@gmail.com</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>+1 630-698-4717</t>
+          <t>+1 669-342-9825</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>https:///linkedin.com/in/esther-hansol-chung-071b9b19b</t>
+          <t>https://www.linkedin.com/in/lydia-chung-98a4671a0/</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>정혜령</t>
+          <t>정휘용</t>
         </is>
       </c>
       <c r="B139" t="inlineStr"/>
@@ -5833,39 +5833,39 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>o</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Samsung Electronics</t>
+          <t>Synopsys</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Sr. Marketing Communications Specialist</t>
+          <t>Director of Sales and Business Development</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>lydia.chung1@gmail.com</t>
+          <t>largon@gmail.com</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>+1 669-342-9825</t>
+          <t>+1 408-497-3022</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/lydia-chung-98a4671a0/</t>
+          <t>https://www.linkedin.com/in/lukehychung/</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>정휘용</t>
+          <t>정희진</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -5881,42 +5881,38 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Synopsys</t>
+          <t>SK hynix</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Director of Sales and Business Development</t>
+          <t>Head of Venture Investment</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>largon@gmail.com</t>
+          <t>heejin.chung@us.skhynix.com</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>+1 408-497-3022</t>
+          <t>+1 408-628-3607</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/lukehychung/</t>
+          <t>https://linkedin.com/in/heejin-chung-3576351</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>정희진</t>
+          <t>조계현</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+      <c r="C141" t="inlineStr"/>
       <c r="D141" t="inlineStr">
         <is>
           <t>o</t>
@@ -5924,194 +5920,198 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>SK hynix</t>
+          <t>MVLASF Holdings</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Head of Venture Investment</t>
+          <t>CEO</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>heejin.chung@us.skhynix.com</t>
+          <t>andrea.jo@mvlasf.com</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>+1 408-628-3607</t>
+          <t>+1 408-220-4041</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>https://linkedin.com/in/heejin-chung-3576351</t>
+          <t>https://www.linkedin.com/in/gyehyon-andrea-jo</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>조계현</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr"/>
-      <c r="C142" t="inlineStr"/>
+          <t>조민선</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>MVLASF Holdings</t>
+          <t>stealth</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>CEO</t>
+          <t>stealth</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>andrea.jo@mvlasf.com</t>
+          <t>christine7597@gmail.com</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>+1 408-220-4041</t>
+          <t>+1 510-561-9348</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/gyehyon-andrea-jo</t>
+          <t>https://www.linkedin.com/in/christine-c-5b8b4b168/</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>조민선</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+          <t>조성정</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="inlineStr"/>
       <c r="D143" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>o</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>stealth</t>
+          <t>Meta</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>stealth</t>
+          <t>Senior Staff SWE</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>christine7597@gmail.com</t>
+          <t>sjcho123@gmail.com</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>+1 510-561-9348</t>
+          <t>+1 650-215-8119</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/christine-c-5b8b4b168/</t>
+          <t>https://www.linkedin.com/in/sjcho</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>조성정</t>
+          <t>조시영</t>
         </is>
       </c>
       <c r="B144" t="inlineStr"/>
       <c r="C144" t="inlineStr"/>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+      <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Meta</t>
+          <t>Keeworks</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Senior Staff SWE</t>
+          <t>Board Member</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>sjcho123@gmail.com</t>
+          <t>siyungj@gmail.com</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
         <is>
-          <t>+1 650-215-8119</t>
-        </is>
-      </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/sjcho</t>
-        </is>
-      </c>
+          <t>+82 10-9459-4385</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>조시영</t>
+          <t>조아라</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
       <c r="C145" t="inlineStr"/>
-      <c r="D145" t="inlineStr"/>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Keeworks</t>
+          <t>Stanford University</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Board Member</t>
+          <t>Postdoctoral Researcher</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>siyungj@gmail.com</t>
+          <t>choara@stanford.edu</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>+82 10-9459-4385</t>
-        </is>
-      </c>
-      <c r="I145" t="inlineStr"/>
+          <t>+1 669-260-4894</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/ara-cho-508b7625b/</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>조아라</t>
+          <t>조정현</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
-      <c r="C146" t="inlineStr"/>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D146" t="inlineStr">
         <is>
           <t>o</t>
@@ -6119,42 +6119,38 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Stanford University</t>
+          <t>Audi of America</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Postdoctoral Researcher</t>
+          <t>ADAS Software Engineer</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>choara@stanford.edu</t>
+          <t>jeonghyunjason@gmail.com</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>+1 669-260-4894</t>
+          <t>+1 415-444-6985</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/ara-cho-508b7625b/</t>
+          <t>https://www.linkedin.com/in/jeonghyunjo/</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>조정현</t>
+          <t>주은광</t>
         </is>
       </c>
       <c r="B147" t="inlineStr"/>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+      <c r="C147" t="inlineStr"/>
       <c r="D147" t="inlineStr">
         <is>
           <t>o</t>
@@ -6162,37 +6158,41 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Audi of America</t>
+          <t>SynStation</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>ADAS Software Engineer</t>
+          <t>CEO</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>jeonghyunjason@gmail.com</t>
+          <t>eugene@wasd3r.xyz</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>+1 415-444-6985</t>
+          <t>+1 510-499-9248</t>
         </is>
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/jeonghyunjo/</t>
+          <t>https:///Linkedin.com/in/ekjoo</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>주은광</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr"/>
+          <t>진승환</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="C148" t="inlineStr"/>
       <c r="D148" t="inlineStr">
         <is>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>SynStation</t>
+          <t>StartupSprintK</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -6211,31 +6211,27 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>eugene@wasd3r.xyz</t>
+          <t>seunghwan.jin@gmail.com</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>+1 510-499-9248</t>
+          <t>+1 650-695-8692</t>
         </is>
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>https:///Linkedin.com/in/ekjoo</t>
+          <t>https://www.linkedin.com/in/seunghwan-jin/</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>진승환</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+          <t>진용진</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr"/>
       <c r="C149" t="inlineStr"/>
       <c r="D149" t="inlineStr">
         <is>
@@ -6244,38 +6240,42 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>StartupSprintK</t>
+          <t>April Labs</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>CEO</t>
+          <t>Product Manager</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>seunghwan.jin@gmail.com</t>
+          <t>yongjin.jin@gmail.com</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>+1 650-695-8692</t>
+          <t>+1 650-289-8487</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/seunghwan-jin/</t>
+          <t>https://www.linkedin.com/in/yongjinjin</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>진용진</t>
+          <t>차동준</t>
         </is>
       </c>
       <c r="B150" t="inlineStr"/>
-      <c r="C150" t="inlineStr"/>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D150" t="inlineStr">
         <is>
           <t>o</t>
@@ -6283,37 +6283,41 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>April Labs</t>
+          <t>Higher Life Ventures</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Product Manager</t>
+          <t>Managing Partner</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>yongjin.jin@gmail.com</t>
+          <t>dongjoon@hlv.vc</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>+1 650-289-8487</t>
+          <t>+1 650-336-4372</t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/yongjinjin</t>
+          <t>https://www.linkedin.com/in/djcha3</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>차동준</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr"/>
+          <t>천정희</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="C151" t="inlineStr">
         <is>
           <t>o</t>
@@ -6321,46 +6325,42 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>x</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Higher Life Ventures</t>
+          <t>CryptoLab Inc.</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>Managing Partner</t>
+          <t>CEO</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>dongjoon@hlv.vc</t>
+          <t>jhcheon@snu.ac.kr</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>+1 650-336-4372</t>
+          <t>+82 10-9767-1912</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/djcha3</t>
+          <t>https://www.linkedin.com/in/jung-hee-cheon-35721918/</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>천정희</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+          <t>최경환</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr"/>
       <c r="C152" t="inlineStr">
         <is>
           <t>o</t>
@@ -6368,199 +6368,199 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>o</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>CryptoLab Inc.</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>CEO</t>
+          <t>Robot Learning Engineer</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>jhcheon@snu.ac.kr</t>
+          <t>choe.kyoung@gmail.com</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
         <is>
-          <t>+82 10-9767-1912</t>
+          <t>+1 872-818-4539</t>
         </is>
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/jung-hee-cheon-35721918/</t>
+          <t>https://www.linkedin.com/in/kywch</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>최경환</t>
+          <t>최영</t>
         </is>
       </c>
       <c r="B153" t="inlineStr"/>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Independent</t>
+          <t>Regent University</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>Robot Learning Engineer</t>
+          <t>Professor</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>choe.kyoung@gmail.com</t>
+          <t>ychoi@regent.edu</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>+1 872-818-4539</t>
-        </is>
-      </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/kywch</t>
-        </is>
-      </c>
+          <t>+1 757-353-4949</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>최영</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr"/>
+          <t>최종록</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="C154" t="inlineStr"/>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Regent University</t>
+          <t>Samsung SDI</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Pro</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>ychoi@regent.edu</t>
+          <t>jongrock@gmail.com</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>+1 757-353-4949</t>
-        </is>
-      </c>
-      <c r="I154" t="inlineStr"/>
+          <t>+1 650-942-1052</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/종록-최-212122246</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>최종록</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr"/>
-      <c r="D155" t="inlineStr"/>
+          <t>최지호</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Samsung SDI</t>
+          <t>Stanford University</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Pro</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>jongrock@gmail.com</t>
+          <t>choejms@stanford.edu</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>+1 650-942-1052</t>
+          <t>+1 650-507-5712</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/종록-최-212122246</t>
+          <t>https://www.linkedin.com/in/jeeho-choe-84a143156/</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>최지호</t>
+          <t>최해준</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+      <c r="C156" t="inlineStr"/>
       <c r="D156" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>o</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Stanford University</t>
+          <t>Electronic Arts</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Software Engineer</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>choejms@stanford.edu</t>
+          <t>haejoonchoi@outlook.com</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>+1 650-507-5712</t>
+          <t>+1 778-899-6669</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/jeeho-choe-84a143156/</t>
+          <t>https:///LinkedIn.com/in/haejoonchoi</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>최해준</t>
+          <t>팽진희</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>
-      <c r="C157" t="inlineStr"/>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D157" t="inlineStr">
         <is>
           <t>o</t>
@@ -6568,42 +6568,34 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Electronic Arts</t>
+          <t>Stanford University</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Graduate Student</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>haejoonchoi@outlook.com</t>
+          <t>jhpaeng@stanford.edu</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>+1 778-899-6669</t>
-        </is>
-      </c>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t>https:///LinkedIn.com/in/haejoonchoi</t>
-        </is>
-      </c>
+          <t>+1 650-512-6379</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>팽진희</t>
+          <t>하영욱</t>
         </is>
       </c>
       <c r="B158" t="inlineStr"/>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+      <c r="C158" t="inlineStr"/>
       <c r="D158" t="inlineStr">
         <is>
           <t>o</t>
@@ -6611,30 +6603,34 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Stanford University</t>
+          <t>Valleyinnovationpartners</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Graduate Student</t>
+          <t>Co-Founder</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>jhpaeng@stanford.edu</t>
+          <t>ywha.p2o.@gmail.com</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>+1 650-512-6379</t>
-        </is>
-      </c>
-      <c r="I158" t="inlineStr"/>
+          <t>+1 408-747-7247</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>https:///www.linkedin.com/in/young-wook-ha</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>하영욱</t>
+          <t>한수정</t>
         </is>
       </c>
       <c r="B159" t="inlineStr"/>
@@ -6646,38 +6642,42 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Valleyinnovationpartners</t>
+          <t>Stanford GSB</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>Co-Founder</t>
+          <t>MBA1</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>ywha.p2o.@gmail.com</t>
+          <t>sjhan26@stanford.edu</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>+1 408-747-7247</t>
+          <t>+1 650-512-7236</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>https:///www.linkedin.com/in/young-wook-ha</t>
+          <t>https:///www.linkedin.com/in/han-soojung</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>한수정</t>
+          <t>허소영</t>
         </is>
       </c>
       <c r="B160" t="inlineStr"/>
-      <c r="C160" t="inlineStr"/>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="D160" t="inlineStr">
         <is>
           <t>o</t>
@@ -6685,104 +6685,100 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Stanford GSB</t>
+          <t>Samsung Semiconductor</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>MBA1</t>
+          <t>Senior Manager</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>sjhan26@stanford.edu</t>
+          <t>sungok0125@gmail.com</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>+1 650-512-7236</t>
+          <t>+1 408-340-4744</t>
         </is>
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>https:///www.linkedin.com/in/han-soojung</t>
+          <t>https:///www.linkedin.com/in/ella-soy-heo</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>허소영</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr"/>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+          <t>허예랑</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Samsung Semiconductor</t>
+          <t>UClone Inc</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>Senior Manager</t>
+          <t>CEO</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>sungok0125@gmail.com</t>
+          <t>danielhur@uclone.net</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>+1 408-340-4744</t>
-        </is>
-      </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>https:///www.linkedin.com/in/ella-soy-heo</t>
-        </is>
-      </c>
+          <t>+1 408-499-6876</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>허예랑</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr"/>
-      <c r="D162" t="inlineStr"/>
+          <t>홍성헌</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr"/>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>UClone Inc</t>
+          <t>Stanford University</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>CEO</t>
+          <t>Graduate Student</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>danielhur@uclone.net</t>
+          <t>wbfprp@stanford.edu</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>+1 408-499-6876</t>
+          <t>+1 650-289-8265</t>
         </is>
       </c>
       <c r="I162" t="inlineStr"/>
@@ -6790,38 +6786,26 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>홍성헌</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr"/>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>Stanford University</t>
-        </is>
-      </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t>Graduate Student</t>
-        </is>
-      </c>
+          <t>홍창기</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr"/>
       <c r="G163" t="inlineStr">
         <is>
-          <t>wbfprp@stanford.edu</t>
+          <t>ck971120@gmail.com</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>+1 650-289-8265</t>
+          <t>+1 408-504-8539</t>
         </is>
       </c>
       <c r="I163" t="inlineStr"/>
@@ -6829,34 +6813,50 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>홍창기</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr"/>
-      <c r="D164" t="inlineStr"/>
-      <c r="E164" t="inlineStr"/>
-      <c r="F164" t="inlineStr"/>
+          <t>황도연</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr"/>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Stanford University</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Graduate Student (Ph.D.)</t>
+        </is>
+      </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>ck971120@gmail.com</t>
+          <t>doyunh@stanford.edu</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>+1 408-504-8539</t>
-        </is>
-      </c>
-      <c r="I164" t="inlineStr"/>
+          <t>+1 650-468-0741</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/doyun-hwang/</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>황도연</t>
+          <t>황민하</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -6870,128 +6870,85 @@
           <t>x</t>
         </is>
       </c>
-      <c r="E165" t="inlineStr">
-        <is>
-          <t>Stanford University</t>
-        </is>
-      </c>
-      <c r="F165" t="inlineStr">
-        <is>
-          <t>Graduate Student (Ph.D.)</t>
-        </is>
-      </c>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr"/>
       <c r="G165" t="inlineStr">
         <is>
-          <t>doyunh@stanford.edu</t>
-        </is>
-      </c>
-      <c r="H165" t="inlineStr">
-        <is>
-          <t>+1 650-468-0741</t>
-        </is>
-      </c>
+          <t>minha.hwang@gmail.com</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr"/>
       <c r="I165" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/doyun-hwang/</t>
+          <t>https:///linkedin.com/in/minha-hwang-7440771</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>황민하</t>
+          <t>황용현</t>
         </is>
       </c>
       <c r="B166" t="inlineStr"/>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E166" t="inlineStr"/>
-      <c r="F166" t="inlineStr"/>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>WeStory</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>CTO</t>
+        </is>
+      </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>minha.hwang@gmail.com</t>
-        </is>
-      </c>
-      <c r="H166" t="inlineStr"/>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>https:///linkedin.com/in/minha-hwang-7440771</t>
-        </is>
-      </c>
+          <t>freeaion@gmail.com</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>+1 949-436-8067</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>황용현</t>
+          <t>황의선</t>
         </is>
       </c>
       <c r="B167" t="inlineStr"/>
       <c r="C167" t="inlineStr"/>
-      <c r="D167" t="inlineStr"/>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>WeStory</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>CTO</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>freeaion@gmail.com</t>
+          <t>euysun@stanford.edu</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>+1 949-436-8067</t>
-        </is>
-      </c>
-      <c r="I167" t="inlineStr"/>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>황의선</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr"/>
-      <c r="C168" t="inlineStr"/>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>Stanford</t>
-        </is>
-      </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G168" t="inlineStr">
-        <is>
-          <t>euysun@stanford.edu</t>
-        </is>
-      </c>
-      <c r="H168" t="inlineStr">
-        <is>
           <t>+1 650-422-4583</t>
         </is>
       </c>
-      <c r="I168" t="inlineStr">
+      <c r="I167" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/euysun-hwang/</t>
         </is>

</xml_diff>